<commit_message>
23/9, no bankcheck, 81%
</commit_message>
<xml_diff>
--- a/Ticker_DataLocal.xlsx
+++ b/Ticker_DataLocal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/easter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8162D825-AF0D-8F46-A263-68CD04282028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF4DA94-CEB4-9C45-A14A-7CB4F7E78786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1321,8 +1321,8 @@
           <cell r="B55">
             <v>15.329549999999999</v>
           </cell>
-          <cell r="C55" t="str">
-            <v>2025-09-22</v>
+          <cell r="C55">
+            <v>45986</v>
           </cell>
           <cell r="E55">
             <v>7.1100003999999994E-2</v>
@@ -1945,8 +1945,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3362,9 +3362,9 @@
         <f>[1]Data!B55</f>
         <v>15.329549999999999</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55">
         <f>[1]Data!C55</f>
-        <v>2025-09-22</v>
+        <v>45986</v>
       </c>
       <c r="D55">
         <f>[1]Data!D55</f>
@@ -3883,8 +3883,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5573,7 +5573,7 @@
       </c>
       <c r="F58" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45922</v>
+        <v>45986</v>
       </c>
       <c r="G58" s="4">
         <f>_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="F74" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45922</v>
+        <v>45986</v>
       </c>
       <c r="G74" s="4">
         <f>_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!D$2:D$74)</f>

</xml_diff>

<commit_message>
ws DataShift to be checked after addinh JB positions
</commit_message>
<xml_diff>
--- a/Ticker_DataLocal.xlsx
+++ b/Ticker_DataLocal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF4DA94-CEB4-9C45-A14A-7CB4F7E78786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5CC7D-9F53-CB40-A803-9D819A05E76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Ticker</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>MVE, SAF</t>
+  </si>
+  <si>
+    <t>JBASML</t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1948,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="150" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -3881,10 +3884,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD35AB8-8038-8C4C-A651-D274FEBDAB5A}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93:H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6572,23 +6575,23 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
-        <f>IF(ISNUMBER(SEARCH(".", Sheet1!A93)),LEFT(Sheet1!A93,LEN(Sheet1!A93)-3),Sheet1!A93)</f>
+        <f>IF(ISNUMBER(SEARCH(".", Sheet1!A94)),LEFT(Sheet1!A94,LEN(Sheet1!A94)-3),Sheet1!A94)</f>
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" si="2"/>
-        <v>EOAN</v>
+        <f>IF(OR(LEFT(B93,3)="MVE",LEFT(B93,3)="SAF"),RIGHT(B93, LEN(B93) - 3),                IF(LEFT(B93,2)="JB",RIGHT(B93,LEN(B93)-2),B93))</f>
+        <v>LOCK</v>
       </c>
       <c r="E93">
         <f>VALUE(_xlfn.XLOOKUP($C93,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>16.88824</v>
+        <v>0</v>
       </c>
       <c r="F93" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C93,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45793</v>
+        <v>0</v>
       </c>
       <c r="G93" s="4">
         <f>_xlfn.XLOOKUP($C93,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6596,28 +6599,28 @@
       </c>
       <c r="H93" s="5">
         <f>VALUE(_xlfn.XLOOKUP($C93,$A$2:$A$74,Sheet1!E$2:E$74))</f>
-        <v>3.6199997999999997E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
-        <f>IF(ISNUMBER(SEARCH(".", Sheet1!A94)),LEFT(Sheet1!A94,LEN(Sheet1!A94)-3),Sheet1!A94)</f>
+        <f>IF(ISNUMBER(SEARCH(".", Sheet1!A95)),LEFT(Sheet1!A95,LEN(Sheet1!A95)-3),Sheet1!A95)</f>
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="2"/>
-        <v>LOCK</v>
+        <f>IF(OR(LEFT(B94,3)="MVE",LEFT(B94,3)="SAF"),RIGHT(B94, LEN(B94) - 3),                IF(LEFT(B94,2)="JB",RIGHT(B94,LEN(B94)-2),B94))</f>
+        <v>ASML</v>
       </c>
       <c r="E94">
         <f>VALUE(_xlfn.XLOOKUP($C94,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>0</v>
+        <v>758</v>
       </c>
       <c r="F94" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C94,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>0</v>
+        <v>45866</v>
       </c>
       <c r="G94" s="4">
         <f>_xlfn.XLOOKUP($C94,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6625,7 +6628,36 @@
       </c>
       <c r="H94" s="5">
         <f>VALUE(_xlfn.XLOOKUP($C94,$A$2:$A$74,Sheet1!E$2:E$74))</f>
-        <v>0</v>
+        <v>9.7999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <f>IF(ISNUMBER(SEARCH(".", Sheet1!A93)),LEFT(Sheet1!A93,LEN(Sheet1!A93)-3),Sheet1!A93)</f>
+        <v>0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>97</v>
+      </c>
+      <c r="C95" t="str">
+        <f>IF(OR(LEFT(B95,3)="MVE",LEFT(B95,3)="SAF"),RIGHT(B95, LEN(B95) - 3),                IF(LEFT(B95,2)="JB",RIGHT(B95,LEN(B95)-2),B95))</f>
+        <v>EOAN</v>
+      </c>
+      <c r="E95">
+        <f>VALUE(_xlfn.XLOOKUP($C95,$A$2:$A$74,Sheet1!B$2:B$74))</f>
+        <v>16.88824</v>
+      </c>
+      <c r="F95" s="4">
+        <f>VALUE(_xlfn.XLOOKUP($C95,$A$2:$A$74,Sheet1!C$2:C$74))</f>
+        <v>45793</v>
+      </c>
+      <c r="G95" s="4">
+        <f>_xlfn.XLOOKUP($C95,$A$2:$A$74,Sheet1!D$2:D$74)</f>
+        <v>0</v>
+      </c>
+      <c r="H95" s="5">
+        <f>VALUE(_xlfn.XLOOKUP($C95,$A$2:$A$74,Sheet1!E$2:E$74))</f>
+        <v>3.6199997999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work OK, .py chain, trades not archived
</commit_message>
<xml_diff>
--- a/Ticker_DataLocal.xlsx
+++ b/Ticker_DataLocal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5CC7D-9F53-CB40-A803-9D819A05E76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D1020B-0EC5-584F-AF86-3945BC48BCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="14400" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1065,7 +1065,7 @@
             <v>RWE.DE</v>
           </cell>
           <cell r="B39">
-            <v>42.911110000000001</v>
+            <v>43.26</v>
           </cell>
           <cell r="C39" t="str">
             <v>2025-05-02</v>
@@ -1322,10 +1322,10 @@
             <v>ENI.MI</v>
           </cell>
           <cell r="B55">
-            <v>15.329549999999999</v>
-          </cell>
-          <cell r="C55">
-            <v>45986</v>
+            <v>15.5</v>
+          </cell>
+          <cell r="C55" t="str">
+            <v>2025-09-22</v>
           </cell>
           <cell r="E55">
             <v>7.1100003999999994E-2</v>
@@ -1538,7 +1538,7 @@
             <v>OXY</v>
           </cell>
           <cell r="B67">
-            <v>50.652169999999998</v>
+            <v>50.78</v>
           </cell>
           <cell r="C67" t="str">
             <v>2025-09-10</v>
@@ -1948,8 +1948,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B39">
         <f>[1]Data!B39</f>
-        <v>42.911110000000001</v>
+        <v>43.26</v>
       </c>
       <c r="C39" t="str">
         <f>[1]Data!C39</f>
@@ -3363,11 +3363,11 @@
       </c>
       <c r="B55">
         <f>[1]Data!B55</f>
-        <v>15.329549999999999</v>
-      </c>
-      <c r="C55">
+        <v>15.5</v>
+      </c>
+      <c r="C55" t="str">
         <f>[1]Data!C55</f>
-        <v>45986</v>
+        <v>2025-09-22</v>
       </c>
       <c r="D55">
         <f>[1]Data!D55</f>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B67">
         <f>[1]Data!B67</f>
-        <v>50.652169999999998</v>
+        <v>50.78</v>
       </c>
       <c r="C67" t="str">
         <f>[1]Data!C67</f>
@@ -3886,8 +3886,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93:H94"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5021,7 +5021,7 @@
       </c>
       <c r="E39">
         <f>VALUE(_xlfn.XLOOKUP($C39,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>42.911110000000001</v>
+        <v>43.26</v>
       </c>
       <c r="F39" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C39,$A$2:$A$74,Sheet1!C$2:C$74))</f>
@@ -5572,11 +5572,11 @@
       </c>
       <c r="E58">
         <f>VALUE(_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>15.329549999999999</v>
+        <v>15.5</v>
       </c>
       <c r="F58" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45986</v>
+        <v>45922</v>
       </c>
       <c r="G58" s="4">
         <f>_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -5688,7 +5688,7 @@
       </c>
       <c r="E62">
         <f>VALUE(_xlfn.XLOOKUP($C62,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>42.911110000000001</v>
+        <v>43.26</v>
       </c>
       <c r="F62" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C62,$A$2:$A$74,Sheet1!C$2:C$74))</f>
@@ -5799,7 +5799,7 @@
         <v>86</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C94" si="2">IF(OR(LEFT(B66,3)="MVE",LEFT(B66,3)="SAF"),RIGHT(B66, LEN(B66) - 3),                IF(LEFT(B66,2)="JB",RIGHT(B66,LEN(B66)-2),B66))</f>
+        <f t="shared" ref="C66:C92" si="2">IF(OR(LEFT(B66,3)="MVE",LEFT(B66,3)="SAF"),RIGHT(B66, LEN(B66) - 3),                IF(LEFT(B66,2)="JB",RIGHT(B66,LEN(B66)-2),B66))</f>
         <v>AMZN</v>
       </c>
       <c r="E66">
@@ -6036,11 +6036,11 @@
       </c>
       <c r="E74">
         <f>VALUE(_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>15.329549999999999</v>
+        <v>15.5</v>
       </c>
       <c r="F74" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45986</v>
+        <v>45922</v>
       </c>
       <c r="G74" s="4">
         <f>_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E86">
         <f>VALUE(_xlfn.XLOOKUP($C86,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>50.652169999999998</v>
+        <v>50.78</v>
       </c>
       <c r="F86" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C86,$A$2:$A$74,Sheet1!C$2:C$74))</f>

</xml_diff>

<commit_message>
8/10, Trapper to repair
</commit_message>
<xml_diff>
--- a/Ticker_DataLocal.xlsx
+++ b/Ticker_DataLocal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A84E5-9C41-1343-A986-BD88B9C92795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171EEB0C-E019-A64A-83CA-000D78B0A372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28820" yWindow="-19600" windowWidth="14400" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1324,8 +1324,8 @@
           <cell r="B55">
             <v>15.5</v>
           </cell>
-          <cell r="C55" t="str">
-            <v>2025-09-22</v>
+          <cell r="C55">
+            <v>45985</v>
           </cell>
           <cell r="E55">
             <v>7.1100003999999994E-2</v>
@@ -1629,7 +1629,7 @@
             <v>THC</v>
           </cell>
           <cell r="B72">
-            <v>197.52379999999999</v>
+            <v>201.43</v>
           </cell>
           <cell r="C72" t="str">
             <v>2000-03-13</v>
@@ -3365,9 +3365,9 @@
         <f>[1]Data!B55</f>
         <v>15.5</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55">
         <f>[1]Data!C55</f>
-        <v>2025-09-22</v>
+        <v>45985</v>
       </c>
       <c r="D55">
         <f>[1]Data!D55</f>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B72">
         <f>[1]Data!B72</f>
-        <v>197.52379999999999</v>
+        <v>201.43</v>
       </c>
       <c r="C72" t="str">
         <f>[1]Data!C72</f>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="F58" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45922</v>
+        <v>45985</v>
       </c>
       <c r="G58" s="4">
         <f>_xlfn.XLOOKUP($C58,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="F74" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!C$2:C$74))</f>
-        <v>45922</v>
+        <v>45985</v>
       </c>
       <c r="G74" s="4">
         <f>_xlfn.XLOOKUP($C74,$A$2:$A$74,Sheet1!D$2:D$74)</f>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="E91">
         <f>VALUE(_xlfn.XLOOKUP($C91,$A$2:$A$74,Sheet1!B$2:B$74))</f>
-        <v>197.52379999999999</v>
+        <v>201.43</v>
       </c>
       <c r="F91" s="4">
         <f>VALUE(_xlfn.XLOOKUP($C91,$A$2:$A$74,Sheet1!C$2:C$74))</f>

</xml_diff>